<commit_message>
The companion website of GenA11y
</commit_message>
<xml_diff>
--- a/WCAG Study/WCAG 2.2 Study.xlsx
+++ b/WCAG Study/WCAG 2.2 Study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD\Project\LLM Accessibility Issues\Companion Website\GenA11y\GenA11y\WCAG Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B003B5-1259-4EC8-8572-CFA017EC4D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FAA02E-51DD-40EE-A37F-E5D08A35117F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:B87"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -570,7 +570,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -802,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -810,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -834,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -858,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -874,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -898,7 +898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -906,7 +906,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -914,7 +914,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -922,7 +922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -930,7 +930,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -938,7 +938,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -946,7 +946,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -954,7 +954,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -962,7 +962,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -970,7 +970,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -978,7 +978,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -986,7 +986,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -994,7 +994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
@@ -1259,6 +1259,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B87">
+    <sortCondition descending="1" ref="B2:B87"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B87" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Static Analysis,Dynamic Analysis,Not Testable,Not Supported"</formula1>

</xml_diff>